<commit_message>
rename files for simplicity update .gitignore to stop tracking data archives
</commit_message>
<xml_diff>
--- a/data_rename.xlsx
+++ b/data_rename.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\ZEN\ZEN-geography\ZEN_geography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A190CC2-7742-4BA4-9454-3BC5D0F6AE01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CEBE1B-19DB-400B-B80E-9A35899B99CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7720" xr2:uid="{FC226BDE-954B-4F17-A2C9-B18E52A45263}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>directory</t>
   </si>
@@ -48,9 +48,6 @@
     <t>ZEN_2011_ZRG_AllSites_Edit141102.csv</t>
   </si>
   <si>
-    <t>ZEN_2014_abund_traits_merge_2016-08-19_copy.csv</t>
-  </si>
-  <si>
     <t>ZEN_2014_data_environmental_20210124_copy.csv</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>ZEN_2014_epibiota_mass_2016_01_06 copy.csv</t>
   </si>
   <si>
-    <t>ZEN_2014_fca_scores_atlantic_20210125_copy.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_fca_scores_pacific_20210125_copy.csv</t>
-  </si>
-  <si>
     <t>ZEN_2014_R_PercentCover_by_plot_2016_01_06_modified_copy.csv</t>
   </si>
   <si>
@@ -75,112 +66,40 @@
     <t>zen_2014_sites copy.csv</t>
   </si>
   <si>
-    <t>archive/ZEN_2014_imputed_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_plot_20210430.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_plot_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_plot_49_Atlantic_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_plot_49_noNA_20210227.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_plot_49_noNA_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_plot_49_Pacific_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_20210315.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_20210315.xlsx</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_49_Atlantic_20210227.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_49_Atlantic_20210314.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_49_Atlantic_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_Atlantic.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_Atlantic_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_Pacific_20210314.csv</t>
-  </si>
-  <si>
-    <t>archive/ZEN_2014_site_means_Pacific_20220529.csv</t>
-  </si>
-  <si>
-    <t>archive/zen2014_imputed.csv</t>
-  </si>
-  <si>
-    <t>archive/zen2014_imputed_49.csv</t>
-  </si>
-  <si>
     <t>data/input</t>
   </si>
   <si>
-    <t>data/ouput</t>
-  </si>
-  <si>
-    <t>where is the code that generates this?</t>
-  </si>
-  <si>
     <t>questions</t>
   </si>
   <si>
-    <t>why so many versions? Can we mint one without all the suffixes?</t>
-  </si>
-  <si>
-    <t>ZEN_2014_clean.csv</t>
-  </si>
-  <si>
     <t>ZEN_2014_FCA_scores.csv</t>
   </si>
   <si>
-    <t>kept the name because it is from another paper</t>
-  </si>
-  <si>
-    <t>ZEN_2014_abund_traits_merge.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_data_environmental.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_DATA_main.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_epibiota_mass.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_R_Predation_by_site.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_FCA_scores_atlantic.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_FCA_scores_pacific.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_R_PercentCover_by_plot.csv</t>
-  </si>
-  <si>
-    <t>ZEN_2014_sites.csv</t>
+    <t>ZEN_2011_ZRG.csv</t>
+  </si>
+  <si>
+    <t>ZEN_2014_main_data.csv</t>
+  </si>
+  <si>
+    <t>Is there script that generates this?</t>
+  </si>
+  <si>
+    <t>ZEN_2014_percent_cover_plot.csv</t>
+  </si>
+  <si>
+    <t>ZEN_2014_predation_site.csv</t>
+  </si>
+  <si>
+    <t>ZEN_2014_epibiota_mass_recalc.csv</t>
+  </si>
+  <si>
+    <t>ZEN_2014_site_metadata.csv</t>
+  </si>
+  <si>
+    <t>ZEN_2014_environmental.csv</t>
+  </si>
+  <si>
+    <t>archived</t>
   </si>
 </sst>
 </file>
@@ -532,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6FBA4A-C3F0-4FC1-9194-8D7AFB876EE1}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -558,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -566,304 +485,113 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>44</v>
+      <c r="E6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>